<commit_message>
Various bug fixes, updated example file
</commit_message>
<xml_diff>
--- a/public/fluxdata_example_file.xlsx
+++ b/public/fluxdata_example_file.xlsx
@@ -932,7 +932,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -965,6 +965,9 @@
       <c r="G1" t="str">
         <v>direction</v>
       </c>
+      <c r="H1" t="str">
+        <v>legend</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -977,7 +980,7 @@
         <v>129</v>
       </c>
       <c r="D2" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -987,6 +990,9 @@
       </c>
       <c r="G2" t="str">
         <v>r</v>
+      </c>
+      <c r="H2" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="3">
@@ -1506,7 +1512,7 @@
         <v>87.8</v>
       </c>
       <c r="D25" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1516,6 +1522,9 @@
       </c>
       <c r="G25" t="str">
         <v>r</v>
+      </c>
+      <c r="H25" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="26">
@@ -1529,7 +1538,7 @@
         <v>11.5</v>
       </c>
       <c r="D26" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1539,6 +1548,9 @@
       </c>
       <c r="G26" t="str">
         <v>r</v>
+      </c>
+      <c r="H26" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="27">
@@ -1552,7 +1564,7 @@
         <v>9.3</v>
       </c>
       <c r="D27" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1562,6 +1574,9 @@
       </c>
       <c r="G27" t="str">
         <v>r</v>
+      </c>
+      <c r="H27" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="28">
@@ -1575,7 +1590,7 @@
         <v>6.6</v>
       </c>
       <c r="D28" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1585,6 +1600,9 @@
       </c>
       <c r="G28" t="str">
         <v>r</v>
+      </c>
+      <c r="H28" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="29">
@@ -1598,7 +1616,7 @@
         <v>5.5</v>
       </c>
       <c r="D29" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1608,6 +1626,9 @@
       </c>
       <c r="G29" t="str">
         <v>r</v>
+      </c>
+      <c r="H29" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="30">
@@ -1621,7 +1642,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1631,6 +1652,9 @@
       </c>
       <c r="G30" t="str">
         <v>r</v>
+      </c>
+      <c r="H30" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="31">
@@ -1644,7 +1668,7 @@
         <v>1.8</v>
       </c>
       <c r="D31" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1654,6 +1678,9 @@
       </c>
       <c r="G31" t="str">
         <v>r</v>
+      </c>
+      <c r="H31" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="32">
@@ -1667,7 +1694,7 @@
         <v>0.6</v>
       </c>
       <c r="D32" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1677,6 +1704,9 @@
       </c>
       <c r="G32" t="str">
         <v>r</v>
+      </c>
+      <c r="H32" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="33">
@@ -1690,7 +1720,7 @@
         <v>0.6</v>
       </c>
       <c r="D33" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1700,6 +1730,9 @@
       </c>
       <c r="G33" t="str">
         <v>r</v>
+      </c>
+      <c r="H33" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="34">
@@ -1713,7 +1746,7 @@
         <v>0.1</v>
       </c>
       <c r="D34" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1723,6 +1756,9 @@
       </c>
       <c r="G34" t="str">
         <v>r</v>
+      </c>
+      <c r="H34" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="35">
@@ -1782,7 +1818,7 @@
         <v>7.7</v>
       </c>
       <c r="D37" t="str">
-        <v>belastingen</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1792,6 +1828,9 @@
       </c>
       <c r="G37" t="str">
         <v>r</v>
+      </c>
+      <c r="H37" t="str">
+        <v>indirecte_belastingen</v>
       </c>
     </row>
     <row r="38">
@@ -1888,7 +1927,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H41"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2759,7 +2798,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2779,55 +2818,47 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>belastingen</v>
+        <v>Premies</v>
       </c>
       <c r="B2" t="str">
-        <v>#3498db</v>
+        <v>#db4c33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Premies</v>
+        <v>Uitgaven</v>
       </c>
       <c r="B3" t="str">
-        <v>#db4c33</v>
+        <v>#73b0af</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Uitgaven</v>
+        <v>Begrotingstekort</v>
       </c>
       <c r="B4" t="str">
-        <v>#73b0af</v>
+        <v>#696969</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Begrotingstekort</v>
+        <v>directe_belasting</v>
       </c>
       <c r="B5" t="str">
-        <v>#696969</v>
+        <v>#a167da</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>directe_belasting</v>
+        <v>indirecte_belastingen</v>
       </c>
       <c r="B6" t="str">
-        <v>#a167da</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>indirecte_belastingen</v>
-      </c>
-      <c r="B7" t="str">
         <v>#3498db</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>